<commit_message>
attempt 1 at deploying backend
</commit_message>
<xml_diff>
--- a/backend/static/user_pulls/output.xlsx
+++ b/backend/static/user_pulls/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Serial No</t>
   </si>
@@ -31,100 +31,139 @@
     <t>Text Summary</t>
   </si>
   <si>
-    <t>DOta2</t>
-  </si>
-  <si>
-    <t>http://www.dota2.com/</t>
-  </si>
-  <si>
-    <t>https://twitter.com/DOTA2?ref_src=twsrc%5Egoogle%7Ctwcamp%5Eserp%7Ctwgr%5Eauthor</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Dota_2</t>
-  </si>
-  <si>
-    <t>https://store.steampowered.com/app/570/Dota_2/</t>
-  </si>
-  <si>
-    <t>https://www.dotabuff.com/</t>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Hello_(Adele_song)</t>
+  </si>
+  <si>
+    <t>https://www.huffpost.com/entry/adele-talks-about-her-son-hello-the-today-show_n_5665d07ee4b072e9d1c6dee7</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/List_of_songs_recorded_by_Adele</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Hello_(Lionel_Richie_song)</t>
+  </si>
+  <si>
+    <t>https://www.azlyrics.com/lyrics/adele/hello.html</t>
+  </si>
+  <si>
+    <t>https://genius.com/Adele-hello-lyrics</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/track/4aebBr4JAihzJQR0CiIZJv</t>
+  </si>
+  <si>
+    <t>https://www.hellomagazine.com/</t>
+  </si>
+  <si>
+    <t>https://supersimple.com/song/hello/</t>
+  </si>
+  <si>
+    <t>https://www.insider.com/hello-from-the-inside-adele-parody-chris-mann-2020-4</t>
+  </si>
+  <si>
+    <t>Hello (Adele song)</t>
   </si>
   <si>
     <t>Title Could not be Retrieved due to Webpage Restrictions</t>
   </si>
   <si>
-    <t xml:space="preserve">
-DOTA 2Verified account
-</t>
-  </si>
-  <si>
-    <t>Dota 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_x000D_
-				Play Dota 2			</t>
-  </si>
-  <si>
-    <t>DOTABUFF</t>
-  </si>
-  <si>
-    <t>Today’s update features a change to the rank system that replaces the Core/Support separation with a single rank that uses handicaps for each of the five ranked roles, representing your relative strength playing each position.
-Queuing for your weaker role(s), however, will result in the matchmaker placing you into a match at a lower MMR.
-Starting after TI10, the Dota Pro Circuit will introduce a new system that presents competitive Dota in a more scheduled and consistent way during the year and features a better structure for the development of Tier 2 and Tier 3 teams.
-Each season will be composed of 6 regional leagues, leading into a Major with the best teams in the world.
-Leagues will feature two divisions with 8 teams in the Upper Division and 8 in the Lower division, for a total of 96 teams participating across the world.
-After each season, the 2 bottom teams of the Upper Division will swap places with the top 2 of the Lower Division.
-The bottom 2 teams of the Lower Division will be eliminated from the league and replaced with 2 new teams coming from Open Qualifiers to allow for new teams and talent to be introduced into the scene over time.
-The leagues will have a duration of six weeks, and each region will consist of a full Bo3 Round Robin among all teams.
-In order to make it easier to follow your favorite region and teams, all matches will be in consistent date and time slots throughout the year for each region.
-Each slot represents a Best of 3 series: For the inaugural season, Valve will allocate the initial teams to the Upper and Lower divisions.
-Additionally, teams will be able to use a stand-in for up to 4 of their matches as long as that stand-in is either competing in a lower division or not competing in a league at all.
-If a team decides to change regions, they will have to enter the region through open qualifiers and climb through that region’s Lower Division.
-The season will conclude with a Major tournament featuring 18 teams from all regions and sporting a prize pool of USD 500,000 plus DPC points.
-The 18 participating teams are the top spots from each regional Upper Division.
-Top two teams advance to the Playoffs upper bracket.
-3rd to 6th place advance to Playoffs lower bracket.
-Group Stage – 2nd place Lower Bracket:
-Group Stage – 6th place At the end of the third season, the top 12 teams with the most DPC points will qualify for The International 2021.
-Join the pros who battled in The International Grand Finals — World Champions OG and runners-up Team Liquid (now the newly-dubbed Nigma) — alongside a live theater audience in Berlin, Germany on January 28th for the world premiere of True Sight: The International 2019.
-Now, fans from around the globe can tune in live on Tuesday, January 28th at 7:00 p.m. CET to see exactly how the story unfolded as the teams themselves relive the epic journey at the world premiere event — hosted by Grand Finals casters ODPixel and Fogged, and joined by The International broadcast stalwarts Kaci and Slacks.</t>
-  </si>
-  <si>
-    <t>Viewing Tweets won't unblock @DOTA2 The 7.25c Gameplay Update has been released https://dota2.com/patches/7.25c The 7.25 Gameplay Update has been released https://dota2.com/patches/7.25 Given the high fluidity of the state of both the pandemic and geopolitical landscape, we will keep following the situation and decide how to approach the final major and minor of the season as the weeks progress.
-Today's update introduces the Treasure of the Fallen Cinder, featuring eleven new item sets — including a rare set for Phoenix and very rare set for Wraith King.pic.twitter.com/hD4KFEqFnU An update to Core/Support MMR http://blog.dota2.com/2020/03/ranked-roles-update/ … Request for Proposals and details on the DPC Season 2020/2021:http://www.dota2.com/procircuit/fall2020 … The 7.24b Gameplay Update has been released https://dota2.com/patches/7.24b Introducing Regional Leagues.
-http://blog.dota2.com/2020/02/introducing-regional-leagues/ …pic.twitter.com/t4O9QY5vwX We have banned over 40,000 accounts for players who were found abusing matchmaking.
-9 2pic.twitter.com/OYji3kjZPk The 7.24 Gameplay Update has been released https://dota2.com/patches/7.24 Just in time for Lunar New Year, the Treasure of Unbound Majesty is now available in the Dota 2 store.
-Claim one for free by completing the New Bloom reward line.pic.twitter.com/n3pzLHVrAV The 7.23f Gameplay Update has been released https://dota2.com/patches/7.23f Join @OGesports and @TeamLiquid (now @nigmagg) for the World Premiere of True Sight, hosted by @ODPixel and @Foggeddota, January 28, 2020!
-Today's update adds Strict Solo Matchmaking option back for fast queue games The 7.23e Gameplay Update has been released https://dota2.com/patches/7.23e @DOTA2 hasn't Tweeted yet.
-Add this Tweet to your website by copying the code below.
-Follow more accounts to get instant updates about topics you care about.</t>
-  </si>
-  <si>
-    <t>Dota 2 is a multiplayer online battle arena (MOBA) video game in which two teams of five players compete to collectively destroy a large structure defended by the opposing team known as the "Ancient", whilst defending their own.[1][2] As in Defense of the Ancients, the game is controlled using standard real-time strategy controls, and is presented on a single map in a three-dimensional isometric perspective.[1][3] Ten players each control one of the game's 119 playable characters, known as "heroes", with each having their own design, strengths, and weaknesses.[1][2][4] Heroes are divided into two primary roles, known as the core and support.[5][6] Cores, which are also called carries, begin each match as weak and vulnerable, but are able to become more powerful later in the game, thus becoming able to "carry" their team to victory.[5][7] Supports generally lack abilities that deal heavy damage, instead having ones with more functionality and utility that provide assistance for their cores, such as providing healing and other buffs.[5][6][8] Players select their hero during a pre-game drafting phase, where they can also discuss potential strategies and hero matchups with their teammates.[2][5][6] Heroes are removed from the drafting pool and become unavailable for all other players once one is selected, and can not be changed once the drafting phase is over.
-Players also receive a continuous, but small stream of gold over the course of a match.[5][16] Multiple game types in the game exist, which mainly alter the way hero selection is handled; examples include "All Pick", which offer no restrictions on hero selection, "All Random", which randomly assigns a hero for each player, "Captain's Mode", where a single player on each team selects heroes for their entire team and is primarily used for professional play, and "Turbo", an expedited version of All Pick featuring increased gold and experience gain, weaker towers, and faster respawn times.[17][18][19] Matches usually last around 30 minutes to an hour, although they can last forever as long as both Ancients remain standing.[6][20] In Captain's Mode games, an additional "GG" forfeit feature is available to end games early.[21] Dota 2 also occasionally features limited-time events that present players with alternative game modes that do not follow the game's standard rules.[22] Some of these included the Halloween-themed Diretide event,[23] the Christmas-themed Frostivus event,[24] and the New Bloom Festival, which celebrated the coming of spring.[25] Other special game modes have also been created by Valve, including a ten-versus-ten mode,[26] a Halloween-themed capture point mode "Colosseum",[27] a combat arena mode "Overthrow",[28] "Siltbreaker", a story-driven cooperative campaign mode,[29] and "The Underhollow", a battle royale mode.[30] The move to the Source 2 engine in 2015 also added the "Arcade" feature, which allows for community-created game modes, with the more popular ones having dedicated server hosting by Valve.[31][32] One popular example, known as Dota Auto Chess, had over seven million in-game subscribers by April 2019.[33][34][35] Due to its popularity, Valve met with the mod's developers, the Chinese-based Drodo Studio, to discuss directly collaborating on a standalone version.
-In the first Q&amp;A session regarding Dota 2, IceFrog explained that the game would build upon the mod without making significant changes to its core.[48] Valve contracted major contributors from the Defense of the Ancients community, including Eul and artist Kendrick Lim, to assist with the sequel.[60] Additional contributions from sources outside of Valve were also sought regularly for Dota 2, as to continue Defense of the Ancients's tradition of community-sourced development.[61] One of the composers of Warcraft III: Reign of Chaos, Jason Hayes, was hired to collaborate with Tim Larkin to write the original score for the game, which was conducted by Timothy Williams and performed and recorded by the Northwest Sinfonia at Bastyr University.[62][63] Valve had Half-Life series writer Marc Laidlaw, science fiction author Ted Kosmatka, and Steam support employee Kris Katz write new dialog and background lore for the heroes.[64][65] Notable voice actors for heroes include Nolan North, Dave Fennoy, Jon St. John, Ellen McLain, Fred Tatasciore, Merle Dandridge, Jen Taylor, and John Patrick Lowrie, among others.[66] The Source engine itself was updated with new features to accommodate Dota 2, such as high-end cloth modeling and improved global lighting.[50] The game features Steam integration, which provides its social component and cloud storage for personal settings.
-Ticket fees are apportioned in part to tournament organizers.[70] The game also features an in-game fantasy sports system, which is modeled after traditional fantasy sports and feature professional Dota 2 players and teams.[71] Players are also able to spectate games in virtual reality (VR) with up to 15 others, which was added in an update in July 2016.[72] The update also added a hero showcase mode, which allows players to see all of the heroes and their cosmetics full-size in virtual reality.[73] As part of a plan to develop Dota 2 into a social network, Newell announced in April 2012 that the game would be free-to-play, and that community contributions would be a cornerstone feature.[74] Instead, revenue is generated through the "Dota Store", which offers for-purchase cosmetic virtual goods, such as custom armor and weapons for their heroes.[75] It was also announced that the full roster of heroes would be available at launch for free.[76] Until the game's official release in 2013, players were able to purchase an early access bundle, which included a digital copy of Dota 2 and several cosmetic items.[77] Included as optional downloadable content (DLC), the Dota 2 Workshop Tools are a set of Source 2 software development kit (SDK) tools that allow content creators to create new hero cosmetics, as well as custom game modes, maps, and bot scripts.[78][79][80] Highly rated cosmetics, through the Steam Workshop, are available in the in-game store if they are accepted by Valve.
-This model was fashioned after Valve's Team Fortress 2, which had earned Workshop designers of cosmetic items of that game over $3.5 million by June 2011.[76] Newell revealed that the average Steam Workshop contributor for Dota 2 and Team Fortess 2 made approximately $15,000 from their creations in 2013.[81] By 2015, sales of Dota 2 virtual goods had earned Valve over $238 million in revenue, according to the digital game market research group SuperData.[82] In 2016, Valve introduced the "Custom Game Pass" option for creators of custom game modes, which allows them to be funded by way of microtransactions by adding exclusive features, content, and other changes to their game mode for players who buy it.[83] Dota 2 includes a seasonal Elo rating-based matchmaking system, which is measured by a numerical value known as "matchmaking rating" (MMR) that is tracked separately for core and support roles, and ranked into different tiers.
-MMR is updated based on if a player won or lost, which will then increase or decrease respectively.[84] The game's servers, known as the "Game Coordinator",[85][86] attempts to balance both teams based on each player's MMR, with each team having roughly a 50% chance to win in any given game.[84] Ranked game modes with a separately tracked MMR are also available, which primarily differ from unranked games by making MMR publicly visible, as well as requiring the registration of a phone number to their accounts, which help foster a more competitive environment.[84][87] To ensure that each player's ranking is up to date and accurate, MMR is recalibrated around every six months.[88][89] Players with the highest possible medal rank are listed by Valve on an online leaderboard, separated into North American, European, Southeast Asian, and Chinese regions.[90] The game also includes a report system, which allows players to punish player behavior that intentionally provides a negative experience.[91] Players who get reported enough or leave several games before they conclude, a practice known as "abandoning", are then placed into low priority matchmaking, which remains on a player's account until they win a specific number of games, and only groups them with other players who also have the same punishment.[92][93] Other features include an improved replay system from Defense of the Ancients, in which a completed game can be downloaded in-client and viewed by anyone at a later time, and the "hero builds" feature, which provide integrated guides created by the community that highlight to the player on how to play their hero.[94] In June 2015, Valve announced that the entirety of Dota 2 would be ported over to their Source 2 game engine in an update called Dota 2 Reborn.[95] Reborn was first released as an opt-in beta update that same month,[96] and officially replaced the original client in September 2015, making it the first game to use the engine.[97] Reborn included a new user interface framework design, ability for custom game modes created by the community, and the full replacement of the original Source engine with Source 2.[98] Largely attributed to technical difficulties players experienced with the update, the global player base experienced a sharp drop of approximately sixteen percent the month following the release of it.[99] However, after various updates and patches, over a million concurrent players were playing again by the beginning of 2016, with that number being the largest in nearly a year.[100] The move to Source 2 also allowed the use of the Vulkan graphics API, which was released as an optional feature in May 2016, making Dota 2 one of the first games to offer it.[101] Dota 2 was first made available to the public at Gamescom in 2011, coinciding with the inaugural International championship, the game's premier esport tournament event.
-Due to that, Valve lifted the non-disclosure agreement and transitioned the game into open beta in September 2011, allowing players to discuss the game and their experiences publicly.[103][104] Following nearly two years of beta testing, Dota 2 was officially released on Steam for Windows on July 9, 2013, and for OS X and Linux on July 18, 2013.[105][106][107] The game did not launch with every hero from Defense of the Ancients.
-In October 2012, Chinese game publisher Perfect World announced they had received distribution rights for the game in the country.[112] The Chinese client also has a region-specific "Low Violence" mode, which censors and changes most depictions of blood, gore, and skulls in order for the game to follow censorship policies of the country.[113][114] In November 2012, a similar publishing deal was made with the South Korea-based game company Nexon to distribute and market the game in the country, as well as in Japan.[115] Three years later, Nexon announced they would no longer be operating servers for Dota 2, with Valve taking over direct distribution and marketing of the game in those regions.[116] In December 2016, Dota 2 was updated to gameplay version 7.00, also known as "The New Journey" update.[117][118][119] Prior to the update, the Dota series had been in version 6.xx for over a decade, marking the first major revision since IceFrog originally took over development of the original mod in the mid 2000s.[119] The New Journey update added and changed numerous features and mechanics of the game, including adding the first original hero not ported over from Defense of the Ancients, a reworked map, a redesigned HUD, a pre-game phase that allows for players to discuss their team strategy, and a "Talent Tree" ability augmentation system.[118][119] In April 2017, Valve announced changes to the game's ranked matchmaking system, with the main one requiring the registration of a unique phone number to a player's account in order to play them, an anti-griefing and smurfing practice they had previously implemented in their first-person shooter game, Counter-Strike: Global Offensive.[87][120] Further changes to the game's matchmaking were brought in an update in November 2017, where the old numerical MMR system was replaced by a seasonal one based on eight ranked tiers that are recalibrated around every six months, a move that brought the game's ranked system closer to ones used in other competitive games such as Global Offensive, StarCraft, and League of Legends.[121][122][123] For most of 2018, Valve decided to handle gameplay balance updates for the game in a different way.
-In addition to offering everything battle passes previously did, Dota Plus added new features such as a hero-specific achievement system that reward players who complete them with exclusive cosmetics, as well as providing hero and game analytics and statistics gathered from thousands of recent games.[126] To ensure that enough Defense of the Ancients players would take up Dota 2 and to promote the game to a new audience, Valve invited sixteen accomplished Defense of the Ancients esports teams to compete at a Dota 2-specific tournament at Gamescom in August 2011, which later became an annually held event known as The International.[127] From The International 2013 onward, its prize pool began to be crowdfunded through a type of in-game battle pass called the "Compendium", which raises money from players buying them and connected lootboxes to get exclusive in-game cosmetics and other bonuses offered through them.[128][129] 25% of all the revenue made from Compendiums go directly to the prize pool, with sales from the 2013 battle pass raising over US$2.8 million, which made it the largest prize pool in esports history at the time.[130][131] Each iteration of The International since then has surpassed the previous one's prize pool, with the most recent one, The International 2019, having one at over $34 million.[132][133] During its beta phase in the early 2010s, several other esport events would begin hosting Dota 2 events, including the Electronic Sports World Cup,[134] DreamHack,[135] World Cyber Games,[136] and ESL.[137] By the end of 2011, Dota 2 was already one of the highest-paying esport games, second only to StarCraft II.[138] At E3 2013, South Korean company Nexon announced the investment of ₩2 billion (approximately US$1.7 million) into local leagues in the country, which coincided with their distribution partnership with Valve for the game.[139] In February 2015, Valve sponsored Dota 2 Asia Championships was held in Shanghai with a prize pool of over $3 million, raised through compendium sales.[140][141] Since then, other Dota 2 Asia Championships have taken place, with it being sometimes being referred to as the "Chinese International".[142][143] In total, professional Dota 2 tournaments had earned teams and players over $100 million by June 2017, with over half of that being awarded at Internationals, making it the highest earning esport game by a margin of nearly $60 million at the time.[144] From late 2015 until early 2017, Valve sponsored a series of smaller-scale, seasonally held tournaments known as the Dota Major Championships, which all had fixed prize pools of US$3 million.[145][146] Their format was based on the tournament series of the same name that Valve also sponsored for their first-person shooter game, Counter-Strike: Global Offensive.
-While the staff selected StarCraft II: Heart of the Swarm, Dota 2 received the majority of the votes distributed between the nine nominees.[211] Dota 2 was later nominated for the best multiplayer game at the 10th British Academy Games Awards in 2014, but lost to Grand Theft Auto V,[212] and was nominated for Esports Game of the Year at The Game Awards at its events from 2015–2019,[213][214][215][216] while winning the award for best MOBA at the 2015 Global Game Awards.[217] The game was also nominated for the community created "Love/Hate Relationship" award at the inaugural Steam Awards in 2016.[218] In the late 2010s, the game was nominated for Choice Video Game at the 2017 Teen Choice Awards,[219] for Esports Game of the Year at the Golden Joystick Awards and NAVGTR Awards,[220][221][222][223][224] and as IGN's best spectator game.[225] A month prior to its official launch, Dota 2 was already the most played game on Steam with a concurrent player count of nearly 330,000, which outweighed the number of players for the rest of platform's top ten most-played games combined.[226][227][228] It remained as the most played game by concurrent players on the platform for four years,[229][230] having a peak of over one million and never dropping below first place for any extended period of time until being surpassed by PlayerUnknown's Battlegrounds in 2017.[231][232][233] Viewership and followings of professional Dota 2 leagues and tournaments are also popular, with peak viewership numbers of some events reaching upwards in the millions.[234][235][236] Some Asian schools and universities, such as the Asia Pacific University of Technology &amp; Innovation in Malaysia, have held courses teaching students the fundamentals and core skills to use for the game.[237][238] Dota 2 has also been a part of multi-sport events in Asia, such as the Asian Indoor and Martial Arts Games and Southeast Asian Games.[239][240] The popularity of Dota 2 led Valve to produce apparel, accessories, figurines, and several other products featuring the heroes and other elements from the game.
-In addition, Valve secured licensing contracts with third-party producers; the first of these deals concerned a Dota 2 themed SteelSeries mousepad, which was announced alongside the game at Gamescom 2011.[241] In September 2012, Weta Workshop, the prop studio that creates the "Aegis of Champions" trophy for winners of The International,[242] announced a product line that would include statues, weapons, and armor based on characters and items from the game.[243] In February 2013, the National Entertainment Collectibles Association announced a new toy line featuring hero-themed action figures at the American International Toy Fair.[244] At Gamescom 2015, an HTC Vive virtual reality (VR) tech demo based around the shopkeeper of the game's item shop was showcased, allowing participants to interact with various items and objects from the game in VR.[245] The demo, known as Secret Shop, was later included the following year on The Lab, Valve's virtual reality compilation game.[246] After the conclusion of The International 2015, Valve awarded the Collector's Aegis of Champions, a brass replica of the Aegis of Champions award trophy, to those with compendiums of 1,000 levels or more.[247] Valve awarded the Collector's Aegis again the following year for The International 2016, as well as selling a limited edition Dota 2 themed HTC Vive virtual reality headset during the event.[248][249] In July 2017, an 18-track official soundtrack was released by Ipecac Recordings, including a version on vinyl.[250] A digital collectible card game based on the universe of Dota 2 and designed by Magic: The Gathering creator Richard Garfield and Valve, Artifact, was released in November 2018.[251][252][253] Promotional tie-ins to other video games and media have been added to Dota 2 since release, including custom Half-Life 2,[254] Bastion,[254] Portal,[255] The Stanley Parable,[256] Rick and Morty,[257] Fallout 4,[258] Deus Ex: Mankind Divided,[259] and Darkest Dungeon[260] announcer packs, which replace the game's default announcer with ones based on those franchises.
-Known as Free to Play, the film follows three players during their time at the first International in 2011.[268] American basketball player Jeremy Lin, who was a media sensation at the time, had a guest appearance in the film, calling the game "a way of life".[269] Lin later compared the game and the esports scene in general to basketball and other traditional sporting events, saying that there was not much of a difference between the two,[270] while also comparing various NBA all-stars, such as Stephen Curry, Kobe Bryant, and LeBron James, to different heroes in the game.[271] Starting in 2016, Valve began producing an episodic documentary series titled True Sight, a spiritual successor to Free to Play.[272] The first three episodes followed the professional teams Evil Geniuses and Fnatic during the Boston Major tournament in late 2016.[272] More episodes were released over the next few years, focusing on the grand finals of several major tournaments, including the International.[273][274][275] Valve have also endorsed cosplay competitions featuring the game's heroes, which take place during downtime at some Dota 2 tournaments and feature prize pools of their own.[276][277][278] Creation of Dota 2-themed animations and CGI videos, mostly created by the community with Source Filmmaker, also take place.[279] Similar to the cosplay competitions, Valve holds short film contests every year at The International, with winners of the competition also being awarded prize money.[280][281] In addition, Valve have created free webcomics featuring some of the heroes, further detailing their background lore.[282][283][284] A physical collection of the comics was released as Dota 2: The Comic Collection by Dark Horse Comics in August 2017.[285] Dota 2 has also been used in machine learning experiments, with the American artificial intelligence research company OpenAI curating a system, known as the OpenAI Five, that allows bots to learn how to play the game at a high skill level entirely through trial-and-error algorithms.</t>
-  </si>
-  <si>
-    <t>Enter up to 375 characters to add a description to your widget: Copy and paste the HTML below into your website to make the above widget appear Sign in to add your own tags to this product.</t>
-  </si>
-  <si>
-    <t>It seems like every patch tweaks the position just enough for a slew of new heroes to be attempted in it, with varying degrees of success.
-Today we would like to have a look through how the role developed over time and where it currently stands.
-We are continuing our series about roles in Dota in an attempt to help new players better understand the game.
-Today we are going to discuss one of the least popular, yet equally important role — hard support.
-Today we would like to take a look at the biggest winners and losers of the latest Dota balance patch.
-We feel like the pub meta has stabilized enough in the past couple of weeks to start discussing heroes that truly shine in the current iteration of the game.
-They described it as: “..a new system that presents competitive Dota in a more scheduled and consistent way during the year and features a better structure for the development of Tier 2 and Tier 3 teams.” Huskar is currently one of the most popular and successful heroes in pubs.
-Mad Moon is no exception and today we would like to have a quick look at some new meta developments.
-Support from Plus members keep Dotabuff running and help enable us to deliver new features for everyone.</t>
+    <t>List of songs recorded by Adele</t>
+  </si>
+  <si>
+    <t>Hello (Lionel Richie song)</t>
+  </si>
+  <si>
+    <t>"Hello" lyrics</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hello!</t>
+  </si>
+  <si>
+    <t>A man's parody of Adele's 'Hello' about being stuck inside is the relatable quarantine humor we all need</t>
+  </si>
+  <si>
+    <t>"Hello" reached number one in a record breaking 36 countries, including the United Kingdom, where it became her second chart topper, following "Someone Like You", and has the largest opening week sales in three years.
+In the United States, "Hello" debuted at the top of the Billboard Hot 100, reigning for 10 consecutive weeks whilst becoming Adele's fourth number-one on the chart and breaking several records, including becoming the first song to sell over a million digital copies in a week.
+By the end of 2015, it had sold 12.3 million units globally (combined sales and track-equivalent streams) and was the year's 7th best-selling single while it stands as one of the best-selling singles of all-time.[3] The accompanying music video was directed by Xavier Dolan and co-stars Adele and Tristan Wilds.
+Neil McCormick from The Daily Telegraph called it "a beautiful song of loss and regret", adding that "it takes a grip on the kind of memory every listener holds somewhere in their heart and merges it with Adele's own drama."[4] Rolling Stone ranked "Hello" at number 6 on its year-end list to find the 50 best songs of 2015.[22] Several publications have commented on similarities in the theme of the song and accompanying video with that of "Hello" by American singer Lionel Richie.[23][24] Three days after its release, the Official Charts Company announced that "Hello" had accumulated 165,000 chart sales in the United Kingdom, of which 156,000 were downloads.[25] "Hello" entered at the top of the UK Singles Chart on 30 October 2015, –  for the week dated 5 November 2015 –  with 333,000 combined sales, of which 259,000 were downloads, making it the biggest selling number-one single on the chart in three years.
+Including streaming sales and excluding The X Factor and Pop Idol winners' singles, major charity campaign records and Christmas number ones, "Hello" was the second biggest selling number one of the 21st century in the UK, beaten only by Shaggy's "It Wasn't Me", which sold 345,000 copies in a week in February 2001.[26] The following week, the song remained at number one after selling a further 121,000 downloads and was streamed 5.78 million times, the same week the song was certified Gold by the BPI.[27] On 20 May 2016, it spent its 30th week in the UK Top 100.
+As of November 2016, the song has sold 918,700 in pure sales.[28] The song also debuted at number one in Belgium, Czech Republic, France, Germany, Greece, Hungary, Ireland, Israel, Italy, Lebanon, Luxembourg, The Netherlands, Norway, Portugal, Scotland, Slovakia, Spain and Switzerland.[29] In Australia, "Hello" entered at the top of the ARIA Singles Chart on 31 October 2015, selling over 59,075 units, which earned the song a gold certification in its first week.
+The song also became the second fastest-selling single of the year, behind Wiz Khalifa's "See You Again".[30] It marked Adele's second number-one single on the ARIA Singles Chart following 2011's "Someone like You".[31] The single stayed atop the chart for a second week and was certified platinum selling over 70,000 units.[30] On 20 March 2017, Hello re-entered the chart at number 50 and has so far been certified 7x platinum for sales over 490,000 units.[32] In New Zealand, the song debuted at number one on the New Zealand singles chart, holding the position the following week and was certified platinum.[33] In the United States, "Hello" debuted at the top of the Billboard Hot 100 on 2 November 2015, for the chart dated 14 November 2015, becoming only the 24th song to debut at number one.
+"Hello" entered at the top of the Digital Songs chart with sales of 1,112,000, becoming the first track to sell over one million digital copies in a single week and almost doubling the record for the most downloads sold in a week, previously held by Flo Rida's "Right Round", which sold 636,000 downloads in the week ending 28 February 2009.
+"Hello" started with 61.6 million US streams, becoming her first number-one song and the second greatest weekly total on the Streaming Songs chart, behind Baauer's "Harlem Shake", which registered 103 million streams on week of 3 March 2013.[34] "Hello" is the first song to sell more than a million digital copies in a single week and the third highest weekly sales total since Nielsen SoundScan began tracking sales in 1991.
+Only Elton John's "Candle in the Wind 1997/Something About the Way You Look Tonight" has sold more in a single week, selling 3.446 million copies in its opening week and 1.212 million copies in its second week.[35] In its second week, "Hello" stayed at number one on the US Billboard Hot 100, selling another 635,000 digital copies marking the third-best digital sales week and the highest for a non-debut week.
+It also equaled the third-longest stay at the summit among all acts.[42] "Hello" debuted at number one on the Canadian Hot 100 on 3 November 2015, for the chart dated 14 November 2015, selling 140,000 copies and outsold Justin Bieber's "Sorry", which sold 40,000 units the same week.</t>
+  </si>
+  <si>
+    <t>In a new interview with Matt Lauer of “Today,” the singer opens up about her new album, “25,” her adorable son, Angelo, and her happy, healthy life.
+But, as Adele explains to Lauer, she experienced terrible writer’s block when she actually sat down to write the album.
+Adele said it’s about “reconnecting.” “‘Hello’ is just about reconnecting with everyone else and myself,” said the 27-year-old singer to Lauer.
+It was just, you know; it’s, in general, just hello to everyone.” Along with the guilt of being a working parent, Adele recently opened up to i-D about how tough it is to actually be a parent.</t>
+  </si>
+  <si>
+    <t>Adele released her second studio album 21 in 2011.[6] In addition to reuniting with writers with whom she had previously worked, the singer collaborated with several new writers and producers.</t>
+  </si>
+  <si>
+    <t>Taken as the third single from his second solo album Can't Slow Down (1983), the song was released in 1984 and reached number one on three Billboard music charts: the pop chart (for two weeks), the R&amp;B chart (for three weeks),[3] and the adult contemporary chart (for six weeks).</t>
+  </si>
+  <si>
+    <t>Hello, can you hear me?</t>
+  </si>
+  <si>
+    <t>[Music Video] Almost five years after her groundbreaking 21, Adele examines the past and tries to right her wrongs on “Hello.” On the surface, the song appears to be about a break-up from long ago, but the song can also be interpreted as Adele’s attempt at reconciliation with her former self.
+In a tweet, Adele called 21 a “break-up record” and 25 a “make-up record.” Adele revealed the broad inspiration for the song: No, it’s not about anyone specifically.
+A day before the release, Zane Lowe interviewed Adele about her future goals, touring, the album, and the “Hello” music video.
+Although “Hello” was released on October 23, 2015, a portion of the song was first featured during a commercial break on the UK’s X Factor on October 18, 2015.
+The accompanying music video broke the Vevo record for the most views in 24 hours with 27.7 million total.
+“Hello” was directed by Xavier Dolan and was the first music video to be shot by IMAX cameras.
+In an interview with i-D, Adele contextualizes “Hello”: The song is about hurting someone’s feelings but it’s also about trying to stay in touch with myself, which sometimes can be a little bit hard to do,“ she explains.
+The way that I feel when I’m not in England, is…” (she pauses) “desperation.
+Adele explained to Us Weekly: “It’s not about anyone specifically.
+It’s also about my fans as well.” and i-D magazine: “The song is about hurting someone’s feelings but it’s also about trying to stay in touch with myself, which sometimes can be a little bit hard to do.
+When I’m away, I really, really miss my life at home.
+When I’m away, I really, really miss my life at home.
+The way that I feel when I’m not in England, is…desperation.
+I get worked up that I’m missing out on things.
+I get worked up that I’m missing out on things.
+So ‘Hello’ is about wanting to be at home and wanting to reach out to everyone I’ve ever hurt—including myself—and apologize for it.” Co-writer Greg Kurstin spoke about writing and recording “Hello” with Adele in an interview: She didn’t want to just go through and write a pop song with any particular formula.
+And again here: “Hello” started with the two of us in a Metropolis Studios writing room together, with me playing chord progressions on a MIDI piano.
+I started laying the chords down for “Hello” while she was singing.
+Then we brought it back into the control room, where we came up with a verse for the song and a temporary chorus that we didn’t think was right.</t>
+  </si>
+  <si>
+    <t>Preview of Spotify Sign up to get unlimited songs and podcasts with occasional ads.</t>
+  </si>
+  <si>
+    <t>Brooklyn Beckham has been missing his family a lot during the coronavirus lockdown as he is...
+As the UK continues to adjust to daily life amid the coronavirus lockdown, it's more...
+The Queen has been one of the many people to celebrate her birthday in lockdown during the...
+Amanda Holden took to Instagram on Tuesday morning to share a sweet photo of her daughter...
+The Duke and Duchess of Cambridge are among thousands of other parents across the nation, who are continuing to educate their children at home following the end of the two-week...
+The Queen has been one of the many people to celebrate her birthday in lockdown during the coronavirus pandemic, but her family made sure that her big day was made...
+Jennifer Lopez paid the sweetest tribute to her stepdaughter Ella on Tuesday as the pre-teen celebrated her 12th birthday in lockdown.
+Taking to Instagram, the Hustlers actress shared some lovely...
+Brooklyn Beckham has been missing his family a lot during the coronavirus lockdown as he is currently self-isolating far away from them in New York, while the rest of the...</t>
+  </si>
+  <si>
+    <t>I’m hungry.
+I’m hungry.
+I’m not so good.
+I’m not so good.</t>
+  </si>
+  <si>
+    <t>"I was just sitting here in my house and I was really frustrated about everything that's going on, so I did this very silly 'My Corona' cover in two hours in my bathroom," he told Insider.
+"It immediately went viral." "I've never experienced anything like it in my entire life," Mann said.
+In his version, Mann sings, "I need toilet paper, toilet paper, toilet paper, I'm out of toilet paper, it's my Corona." "It was so much fun to do and figure out a way to dance your way through this quarantine," he said.
+"I had the idea to do 'Hello' because it is so melodramatic and serious." "I thought it would be hilarious to do with personal lyrics about what we are feeling in my house, about what it's like to have not been outside, not have seen your friends, and not eat out.
+Mann said it only took him an hour to rewrite the lyrics, which includes funny lines like "Hello, it's me.
+The "Hello" parody video, which was uploaded on March 26, has turned out to be Mann's most popular video to date, with more than 6 million views at the time of writing.
+I'm going to take some time off and enjoy life inside," he said.</t>
   </si>
 </sst>
 </file>
@@ -498,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -539,10 +578,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -556,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -573,10 +612,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -590,10 +629,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -607,10 +646,95 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -620,6 +744,11 @@
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>